<commit_message>
Connector for DC bus is added.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Board Connectors/Connectors.xlsx
+++ b/Project/3501/Furkan/Board Connectors/Connectors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Kart Tarafı</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>CONN TERM RECT TONG 14-16 AWG #8</t>
+  </si>
+  <si>
+    <t>SMD BLOCKM 3 X 7 MM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/wurth-electronics-inc/7466303R/732-10895-2-ND/6643991</t>
+  </si>
+  <si>
+    <t>Surface Mount</t>
+  </si>
+  <si>
+    <t>5 x 7</t>
   </si>
 </sst>
 </file>
@@ -189,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -206,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -470,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,13 +630,27 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H7">
         <v>0</v>
       </c>
@@ -635,8 +661,12 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H8">
         <v>0</v>
       </c>
@@ -757,8 +787,10 @@
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="G5" r:id="rId5"/>
     <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="G7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Weekly report is added.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Board Connectors/Connectors.xlsx
+++ b/Project/3501/Furkan/Board Connectors/Connectors.xlsx
@@ -201,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DSP code is renewed with ADC.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Board Connectors/Connectors.xlsx
+++ b/Project/3501/Furkan/Board Connectors/Connectors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>